<commit_message>
update figure 2 with multiple panels
</commit_message>
<xml_diff>
--- a/data/ms2_fragments.xlsx
+++ b/data/ms2_fragments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/GDrive/projects/acidosgrowth/data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/GDrive/science/manuscripts/20210201 e. agg paper/2021_halamka_et_al/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A326D6-2E16-DD45-A1AD-A074F4012723}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673C685-A39A-8B4C-B0A7-A6733E21ECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24700" yWindow="460" windowWidth="26500" windowHeight="18620" xr2:uid="{2A9B51F8-8D68-F448-8848-A6216E1C99E3}"/>
   </bookViews>
@@ -33,26 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={D3C3C691-0701-6D4D-93FD-71916F511E38}</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D3C3C691-0701-6D4D-93FD-71916F511E38}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    To 1 decimal</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>label</t>
   </si>
@@ -181,6 +163,27 @@
   </si>
   <si>
     <t>C_{51}H_{105}O_6</t>
+  </si>
+  <si>
+    <t>molecular_ion</t>
+  </si>
+  <si>
+    <t>M+H-H_2O</t>
+  </si>
+  <si>
+    <t>C_{64}H_{133}O_{5}</t>
+  </si>
+  <si>
+    <t>M+H-C_{30}H_{58}-2\,H_2O</t>
+  </si>
+  <si>
+    <t>C_{36}H_{71}O_4</t>
+  </si>
+  <si>
+    <t>C_{63}H_{125}O_5</t>
+  </si>
+  <si>
+    <t>M+H-C_{3}H_{4}O_{1}</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,25 +207,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,12 +234,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,9 +256,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Sebastian Kopf" id="{9D4E9D02-E17A-674A-A707-58FB3035AED6}" userId="S::seko0922@colorado.edu::bdcab35a-55d0-461b-af87-1262910168ae" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,35 +554,29 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2021-03-08T05:48:41.57" personId="{9D4E9D02-E17A-674A-A707-58FB3035AED6}" id="{D3C3C691-0701-6D4D-93FD-71916F511E38}">
-    <text>To 1 decimal</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7C4F9D-EB26-5347-95F7-3F8EFDEDD3C1}">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7C4F9D-EB26-5347-95F7-3F8EFDEDD3C1}">
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="171" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -599,14 +586,17 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1024</v>
       </c>
       <c r="C2" t="s">
@@ -618,12 +608,15 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1022</v>
       </c>
       <c r="C3" t="s">
@@ -635,12 +628,15 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1018</v>
       </c>
       <c r="C4" t="s">
@@ -652,356 +648,478 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
-        <v>948</v>
+      <c r="B5" s="2">
+        <v>1004</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
+        <v>962</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>948</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
         <v>943.9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>813.8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4">
-        <v>739.8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
+        <v>813.8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>739.8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
         <v>721.8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B12" s="2">
         <v>603.6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3">
-        <v>585.5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3">
-        <v>581.5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
       <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
-        <v>529.5</v>
+      <c r="B13" s="2">
+        <v>585.5</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3">
-        <v>525.5</v>
+      <c r="B14" s="2">
+        <v>581.5</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3">
-        <v>511.5</v>
+      <c r="B15" s="2">
+        <v>567.5</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3">
-        <v>511.5</v>
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>529.5</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="3">
-        <v>507.5</v>
+      <c r="B17" s="2">
+        <v>525.5</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
+        <v>511.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>511.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2">
+        <v>507.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
         <v>493.5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="3">
-        <v>489.5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3">
-        <v>475.5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3">
-        <v>475.5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
       <c r="E21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
+        <v>489.5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2">
         <v>475.5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="3">
-        <v>471.5</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
+        <v>475.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2">
+        <v>475.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2">
+        <v>471.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
         <v>303.3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="E24" t="b">
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>